<commit_message>
updated insert word list.  added bonus question.
</commit_message>
<xml_diff>
--- a/textmsg_analysis/counts_percents_normedcounts.xlsx
+++ b/textmsg_analysis/counts_percents_normedcounts.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace_courses\LING521\textmsg_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06A0E46-06DD-47C7-82B6-D442441F157B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136D43CE-8FDD-4326-B93B-C0665C65DCD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16980" yWindow="-16620" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A324FF67-DED3-4CE2-8D0E-5DD7F60BEB27}"/>
+    <workbookView xWindow="-16980" yWindow="-16620" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{A324FF67-DED3-4CE2-8D0E-5DD7F60BEB27}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial" sheetId="3" r:id="rId1"/>
     <sheet name="Instructors" sheetId="1" r:id="rId2"/>
     <sheet name="Student (Stopwords)" sheetId="2" r:id="rId3"/>
     <sheet name="Student (Functor)" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Lexical Words (Only)" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="27">
   <si>
     <t>Text message analysis 2007 - October 6, 2019</t>
   </si>
@@ -107,6 +108,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -232,6 +242,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -241,7 +252,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1160,7 +1170,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>360</c:v>
+                  <c:v>658.53658536585374</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1202,7 +1212,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>120</c:v>
+                  <c:v>219.51219512195121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,7 +1254,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>73.170731707317074</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,7 +1296,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>26.666666666666668</c:v>
+                  <c:v>48.780487804878049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2684,6 +2694,814 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15217191601049868"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.55178018372703408"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lexical Words (Only)'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nouns</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Lexical Words (Only)'!$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>360</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-35C0-4B43-ACF6-C2996C2F8045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lexical Words (Only)'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>verbs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Lexical Words (Only)'!$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-35C0-4B43-ACF6-C2996C2F8045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lexical Words (Only)'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adj</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Lexical Words (Only)'!$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-35C0-4B43-ACF6-C2996C2F8045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lexical Words (Only)'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Lexical Words (Only)'!$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>26.666666666666668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-35C0-4B43-ACF6-C2996C2F8045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="562302735"/>
+        <c:axId val="110723807"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="562302735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="110723807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="110723807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562302735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.7314208045422893"/>
+          <c:y val="0.32115169257781989"/>
+          <c:w val="0.22783464566929135"/>
+          <c:h val="0.43539939928522547"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15217191601049868"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.55178018372703408"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Instructors!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nouns</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Instructors!$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>302.08333333333331</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4716-45CA-BD0D-6E2EB3943B03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Instructors!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>verbs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Instructors!$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>145.83333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4716-45CA-BD0D-6E2EB3943B03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Instructors!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adj</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Instructors!$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10.416666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4716-45CA-BD0D-6E2EB3943B03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Instructors!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Instructors!$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>62.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4716-45CA-BD0D-6E2EB3943B03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="562302735"/>
+        <c:axId val="110723807"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="562302735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="110723807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="110723807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562302735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.73226908983565309"/>
+          <c:y val="0.29988024790313983"/>
+          <c:w val="0.21182578339076805"/>
+          <c:h val="0.51574946212228712"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2924,6 +3742,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -5450,6 +6348,1016 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6050,7 +7958,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6082,13 +7990,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>47623</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>619126</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6114,6 +8022,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>532992</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{561AD369-5F7E-40C2-80B9-ADC54B053011}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="419100"/>
+          <a:ext cx="3266667" cy="3933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6195,6 +8147,131 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B4F01CF-BFE6-4DE4-9AE8-79245846D686}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47623</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>619126</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4A42B8D-BD35-4038-BD11-92D54D6E431B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>180567</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C4D43B4-7AB6-417A-B4F9-B8AF08987427}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13030200" y="238125"/>
+          <a:ext cx="3266667" cy="3933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6662,21 +8739,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="34.15" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -6819,10 +8896,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3D0190-B52C-48F2-9E7E-AB856EFD7586}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6830,31 +8907,35 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="4" width="9.06640625" style="1"/>
+    <col min="15" max="15" width="11.73046875" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
+    <col min="18" max="18" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="34.15" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:18" ht="34.15" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -6867,8 +8948,17 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="O4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -6876,15 +8966,25 @@
         <v>27</v>
       </c>
       <c r="C5" s="1">
-        <f xml:space="preserve"> B5 / B$11 * 100</f>
-        <v>36</v>
+        <f xml:space="preserve"> B5 / B$9 * 100</f>
+        <v>65.853658536585371</v>
       </c>
       <c r="D5" s="1">
-        <f>B5 / B$11 * 1000</f>
-        <v>360</v>
+        <f>B5 / B$9 * 1000</f>
+        <v>658.53658536585374</v>
+      </c>
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5">
+        <v>145</v>
+      </c>
+      <c r="Q5" s="4">
+        <f xml:space="preserve"> P5 / P9</f>
+        <v>0.40845070422535212</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -6892,15 +8992,25 @@
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <f xml:space="preserve"> B6 / B$11 * 100</f>
-        <v>12</v>
+        <f xml:space="preserve"> B6 / B$9 * 100</f>
+        <v>21.951219512195124</v>
       </c>
       <c r="D6" s="1">
-        <f>B6 / B$11 * 1000</f>
-        <v>120</v>
+        <f>B6 / B$9 * 1000</f>
+        <v>219.51219512195121</v>
+      </c>
+      <c r="O6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6">
+        <v>115</v>
+      </c>
+      <c r="Q6" s="4">
+        <f xml:space="preserve"> P6 / P9</f>
+        <v>0.323943661971831</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -6908,15 +9018,25 @@
         <v>3</v>
       </c>
       <c r="C7" s="1">
-        <f xml:space="preserve"> B7 / B$11 * 100</f>
-        <v>4</v>
+        <f xml:space="preserve"> B7 / B$9 * 100</f>
+        <v>7.3170731707317067</v>
       </c>
       <c r="D7" s="1">
-        <f>B7 / B$11 * 1000</f>
+        <f>B7 / B$9 * 1000</f>
+        <v>73.170731707317074</v>
+      </c>
+      <c r="O7" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7">
         <v>40</v>
       </c>
+      <c r="Q7" s="4">
+        <f xml:space="preserve"> P7 / P9</f>
+        <v>0.11267605633802817</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -6924,211 +9044,187 @@
         <v>2</v>
       </c>
       <c r="C8" s="1">
-        <f xml:space="preserve"> B8 / B$11 * 100</f>
-        <v>2.666666666666667</v>
+        <f xml:space="preserve"> B8 / B$9 * 100</f>
+        <v>4.8780487804878048</v>
       </c>
       <c r="D8" s="1">
-        <f>B8 / B$11 * 1000</f>
-        <v>26.666666666666668</v>
+        <f>B8 / B$9 * 1000</f>
+        <v>48.780487804878049</v>
+      </c>
+      <c r="O8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8">
+        <v>55</v>
+      </c>
+      <c r="Q8" s="4">
+        <f xml:space="preserve"> P8 / P9</f>
+        <v>0.15492957746478872</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="B9" s="1">
-        <v>31</v>
+        <f>SUM(B5:B8)</f>
+        <v>41</v>
       </c>
       <c r="C9" s="1">
-        <f xml:space="preserve"> B9 / B$11 * 100</f>
-        <v>41.333333333333336</v>
+        <f>SUM(C5:C8)</f>
+        <v>100</v>
       </c>
       <c r="D9" s="1">
-        <f>B9 / B$11 * 1000</f>
-        <v>413.33333333333331</v>
+        <f>SUM(D5:D8)</f>
+        <v>1000</v>
+      </c>
+      <c r="P9">
+        <f>SUM(P5:P8)</f>
+        <v>355</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="13" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:18" ht="34.15" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="7"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1">
+        <f xml:space="preserve"> B18 / B$9 * 100</f>
+        <v>48.780487804878049</v>
+      </c>
+      <c r="D18" s="1">
+        <f>B18 / B$9 * 1000</f>
+        <v>487.80487804878049</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" ref="C19:C22" si="0" xml:space="preserve"> B19 / B$9 * 100</f>
+        <v>34.146341463414636</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" ref="D19:D22" si="1">B19 / B$9 * 1000</f>
+        <v>341.46341463414637</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4390243902439024</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
+        <v>24.390243902439025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1">
-        <f xml:space="preserve"> B10 / B$11 * 100</f>
-        <v>4</v>
-      </c>
-      <c r="D10" s="1">
-        <f>B10 / B$11 * 1000</f>
-        <v>40</v>
-      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>14.634146341463413</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>146.34146341463415</v>
+      </c>
+      <c r="S21" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B11" s="1">
-        <f>SUM(B5:B10)</f>
-        <v>75</v>
-      </c>
-      <c r="C11" s="1">
-        <f>SUM(C5:C10)</f>
-        <v>100</v>
-      </c>
-      <c r="D11" s="1">
-        <f>SUM(D5:D10)</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="16" spans="1:13" ht="34.15" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="A16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1">
-        <v>20</v>
-      </c>
-      <c r="C20" s="1">
-        <f xml:space="preserve"> B20 / B$11 * 100</f>
-        <v>26.666666666666668</v>
-      </c>
-      <c r="D20" s="1">
-        <f>B20 / B$11 * 1000</f>
-        <v>266.66666666666669</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1">
-        <v>14</v>
-      </c>
-      <c r="C21" s="1">
-        <f t="shared" ref="C21:C26" si="0" xml:space="preserve"> B21 / B$11 * 100</f>
-        <v>18.666666666666668</v>
-      </c>
-      <c r="D21" s="1">
-        <f t="shared" ref="D21:D26" si="1">B21 / B$11 * 1000</f>
-        <v>186.66666666666669</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B22" s="1">
-        <v>1</v>
+        <f>SUM(B18:B21)</f>
+        <v>41</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
-        <v>1.3333333333333335</v>
+        <v>100</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="1"/>
-        <v>13.333333333333334</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1">
-        <v>31</v>
-      </c>
-      <c r="C24" s="1">
-        <f t="shared" si="0"/>
-        <v>41.333333333333336</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" si="1"/>
-        <v>413.33333333333331</v>
-      </c>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="R25" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="1">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3333333333333339</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" si="1"/>
-        <v>53.333333333333336</v>
-      </c>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="R26" s="4"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B26" s="1">
-        <f>SUM(B20:B25)</f>
-        <v>76</v>
-      </c>
-      <c r="C26" s="1">
-        <f t="shared" si="0"/>
-        <v>101.33333333333334</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="1"/>
-        <v>1013.3333333333334</v>
-      </c>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="R27" s="4"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="R28" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="A14:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7152,21 +9248,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="34.15" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -7195,11 +9291,11 @@
         <v>27</v>
       </c>
       <c r="C5" s="1">
-        <f xml:space="preserve"> B5 / B$11 * 100</f>
+        <f t="shared" ref="C5:C10" si="0" xml:space="preserve"> B5 / B$11 * 100</f>
         <v>36</v>
       </c>
       <c r="D5" s="1">
-        <f>B5 / B$11 * 1000</f>
+        <f t="shared" ref="D5:D10" si="1">B5 / B$11 * 1000</f>
         <v>360</v>
       </c>
     </row>
@@ -7211,11 +9307,11 @@
         <v>12</v>
       </c>
       <c r="C6" s="1">
-        <f xml:space="preserve"> B6 / B$11 * 100</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D6" s="1">
-        <f>B6 / B$11 * 1000</f>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
     </row>
@@ -7227,11 +9323,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="1">
-        <f xml:space="preserve"> B7 / B$11 * 100</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D7" s="1">
-        <f>B7 / B$11 * 1000</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
@@ -7243,11 +9339,11 @@
         <v>7</v>
       </c>
       <c r="C8" s="1">
-        <f xml:space="preserve"> B8 / B$11 * 100</f>
+        <f t="shared" si="0"/>
         <v>9.3333333333333339</v>
       </c>
       <c r="D8" s="1">
-        <f>B8 / B$11 * 1000</f>
+        <f t="shared" si="1"/>
         <v>93.333333333333343</v>
       </c>
     </row>
@@ -7259,11 +9355,11 @@
         <v>23</v>
       </c>
       <c r="C9" s="1">
-        <f xml:space="preserve"> B9 / B$11 * 100</f>
+        <f t="shared" si="0"/>
         <v>30.666666666666664</v>
       </c>
       <c r="D9" s="1">
-        <f>B9 / B$11 * 1000</f>
+        <f t="shared" si="1"/>
         <v>306.66666666666663</v>
       </c>
     </row>
@@ -7275,11 +9371,11 @@
         <v>3</v>
       </c>
       <c r="C10" s="1">
-        <f xml:space="preserve"> B10 / B$11 * 100</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D10" s="1">
-        <f>B10 / B$11 * 1000</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
@@ -7299,21 +9395,21 @@
     </row>
     <row r="15" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="16" spans="1:13" ht="34.15" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
@@ -7358,11 +9454,11 @@
         <v>14</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" ref="C21:C26" si="0" xml:space="preserve"> B21 / B$11 * 100</f>
+        <f t="shared" ref="C21:C26" si="2" xml:space="preserve"> B21 / B$11 * 100</f>
         <v>18.666666666666668</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" ref="D21:D26" si="1">B21 / B$11 * 1000</f>
+        <f t="shared" ref="D21:D26" si="3">B21 / B$11 * 1000</f>
         <v>186.66666666666669</v>
       </c>
     </row>
@@ -7374,11 +9470,11 @@
         <v>1</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.3333333333333335</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13.333333333333334</v>
       </c>
     </row>
@@ -7390,11 +9486,11 @@
         <v>6</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
     </row>
@@ -7406,11 +9502,11 @@
         <v>31</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>41.333333333333336</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>413.33333333333331</v>
       </c>
     </row>
@@ -7422,11 +9518,11 @@
         <v>4</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.3333333333333339</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>53.333333333333336</v>
       </c>
     </row>
@@ -7436,11 +9532,11 @@
         <v>76</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101.33333333333334</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1013.3333333333334</v>
       </c>
     </row>
@@ -7456,11 +9552,446 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CD0D68-1297-4484-B4F4-F7FB5F5E4D12}">
+  <dimension ref="A1:S27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="3" max="4" width="9.06640625" style="1"/>
+    <col min="16" max="16" width="11.46484375" customWidth="1"/>
+    <col min="17" max="17" width="7.06640625" customWidth="1"/>
+    <col min="18" max="18" width="10.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="34.15" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:18" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1">
+        <f xml:space="preserve"> B5 / B$11 * 100</f>
+        <v>36</v>
+      </c>
+      <c r="D5" s="1">
+        <f>B5 / B$11 * 1000</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <f xml:space="preserve"> B6 / B$11 * 100</f>
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6 / B$11 * 1000</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <f xml:space="preserve"> B7 / B$11 * 100</f>
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <f>B7 / B$11 * 1000</f>
+        <v>40</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <f xml:space="preserve"> B8 / B$11 * 100</f>
+        <v>2.666666666666667</v>
+      </c>
+      <c r="D8" s="1">
+        <f>B8 / B$11 * 1000</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="P8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8">
+        <v>145</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0.40849999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" ref="C9:C10" si="0" xml:space="preserve"> B9 / B$11 * 100</f>
+        <v>41.333333333333336</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" ref="D9:D10" si="1">B9 / B$11 * 1000</f>
+        <v>413.33333333333331</v>
+      </c>
+      <c r="P9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9">
+        <v>115</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0.32390000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="P10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10">
+        <v>40</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0.11269999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B11" s="1">
+        <f>SUM(B5:B10)</f>
+        <v>75</v>
+      </c>
+      <c r="C11" s="1">
+        <f>SUM(C5:C10)</f>
+        <v>100</v>
+      </c>
+      <c r="D11" s="1">
+        <f>SUM(D5:D10)</f>
+        <v>1000</v>
+      </c>
+      <c r="P11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11">
+        <v>55</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0.15490000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="16" spans="1:18" ht="34.15" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:19" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <f xml:space="preserve"> B20 / B$11 * 100</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="D20" s="1">
+        <f>B20 / B$11 * 1000</f>
+        <v>266.66666666666669</v>
+      </c>
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1">
+        <f xml:space="preserve"> B21 / B$11 * 100</f>
+        <v>18.666666666666668</v>
+      </c>
+      <c r="D21" s="1">
+        <f>B21 / B$11 * 1000</f>
+        <v>186.66666666666669</v>
+      </c>
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <f xml:space="preserve"> B22 / B$11 * 100</f>
+        <v>1.3333333333333335</v>
+      </c>
+      <c r="D22" s="1">
+        <f>B22 / B$11 * 1000</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1">
+        <f xml:space="preserve"> B23 / B$11 * 100</f>
+        <v>8</v>
+      </c>
+      <c r="D23" s="1">
+        <f>B23 / B$11 * 1000</f>
+        <v>80</v>
+      </c>
+      <c r="P23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>20</v>
+      </c>
+      <c r="R23" s="1">
+        <f xml:space="preserve"> Q23 / Q$27 * 100</f>
+        <v>48.780487804878049</v>
+      </c>
+      <c r="S23" s="1">
+        <f>Q23 / Q$11 * 1000</f>
+        <v>363.63636363636363</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1">
+        <f xml:space="preserve"> B24 / B$11 * 100</f>
+        <v>41.333333333333336</v>
+      </c>
+      <c r="D24" s="1">
+        <f>B24 / B$11 * 1000</f>
+        <v>413.33333333333331</v>
+      </c>
+      <c r="P24" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>14</v>
+      </c>
+      <c r="R24" s="1">
+        <f xml:space="preserve"> Q24 / Q$27 * 100</f>
+        <v>34.146341463414636</v>
+      </c>
+      <c r="S24" s="1">
+        <f>Q24 / Q$11 * 1000</f>
+        <v>254.54545454545453</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <f xml:space="preserve"> B25 / B$11 * 100</f>
+        <v>5.3333333333333339</v>
+      </c>
+      <c r="D25" s="1">
+        <f>B25 / B$11 * 1000</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="P25" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1">
+        <f xml:space="preserve"> Q25 / Q$27 * 100</f>
+        <v>2.4390243902439024</v>
+      </c>
+      <c r="S25" s="1">
+        <f>Q25 / Q$11 * 1000</f>
+        <v>18.18181818181818</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="B26" s="1">
+        <f>SUM(B20:B25)</f>
+        <v>76</v>
+      </c>
+      <c r="C26" s="1">
+        <f xml:space="preserve"> B26 / B$11 * 100</f>
+        <v>101.33333333333334</v>
+      </c>
+      <c r="D26" s="1">
+        <f>B26 / B$11 * 1000</f>
+        <v>1013.3333333333334</v>
+      </c>
+      <c r="P26" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>6</v>
+      </c>
+      <c r="R26" s="1">
+        <f xml:space="preserve"> Q26 / Q$27 * 100</f>
+        <v>14.634146341463413</v>
+      </c>
+      <c r="S26" s="1">
+        <f>Q26 / Q$11 * 1000</f>
+        <v>109.09090909090908</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="Q27" s="1">
+        <f>SUM(Q23:Q26)</f>
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A16:M16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B04AD2D-3B7B-411B-A382-C3FBD38894A4}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7492,7 +10023,7 @@
       <c r="B2">
         <v>27</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="4">
         <v>0.32900000000000001</v>
       </c>
       <c r="D2">
@@ -7506,7 +10037,7 @@
       <c r="B3">
         <v>9</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="4">
         <v>0.11</v>
       </c>
       <c r="D3">
@@ -7520,7 +10051,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="D4">
@@ -7534,7 +10065,7 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="4">
         <v>2.4E-2</v>
       </c>
       <c r="D5">
@@ -7548,7 +10079,7 @@
       <c r="B6">
         <v>31</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>0.378</v>
       </c>
       <c r="D6">
@@ -7562,7 +10093,7 @@
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="4">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="D7">
@@ -7574,7 +10105,7 @@
         <f>SUM(B2:B7)</f>
         <v>75</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="4">
         <f>SUM(C2:C7)</f>
         <v>0.91500000000000004</v>
       </c>
@@ -7584,7 +10115,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C9" s="7"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -7593,7 +10124,7 @@
       <c r="B10">
         <v>75</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <v>0.91500000000000004</v>
       </c>
       <c r="D10">

</xml_diff>